<commit_message>
report + fix skenario
</commit_message>
<xml_diff>
--- a/configuration/ForumDiscussion.xlsx
+++ b/configuration/ForumDiscussion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\file\Kuliah\Softtest\Project\CodeMain\SoftwareTesting\configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WILLIAM\OneDrive\Documents\s1Informatika\Semester_5\Softes\project\SoftwareTesting\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E61965-DC6B-43D6-8D3A-6A08CCBB30A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B094AD4-DC53-4619-AF0D-04A9C6DCF98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="8964" xr2:uid="{08FE5855-BE64-4BCC-A401-1E40CDA1582A}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{08FE5855-BE64-4BCC-A401-1E40CDA1582A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>this lms is very laggy</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60827466-E91E-4EDE-AFAD-A0077127B410}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,7 +435,7 @@
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,10 +446,13 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -454,10 +463,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -468,6 +480,9 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>